<commit_message>
Login tests and ProductsTests preparations
</commit_message>
<xml_diff>
--- a/Data/Katalon data.xlsx
+++ b/Data/Katalon data.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RedMonster\eclipse-workspace\Katalon practice\Katalon-practice\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EF05B27-1389-4FFD-B3DF-1140051FA418}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E96740-E375-4E80-B303-EE8D359E0E9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{0F2C6372-01A3-4AE2-8DDF-A837FC85BCF3}"/>
+    <workbookView xWindow="900" yWindow="1770" windowWidth="15375" windowHeight="7890" firstSheet="1" activeTab="3" xr2:uid="{0F2C6372-01A3-4AE2-8DDF-A837FC85BCF3}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="WrongCredentials" sheetId="2" r:id="rId2"/>
     <sheet name="WrongPassword" sheetId="3" r:id="rId3"/>
-    <sheet name="WrongUserName" sheetId="4" r:id="rId4"/>
+    <sheet name="WrongUsername" sheetId="4" r:id="rId4"/>
     <sheet name="NoInput" sheetId="5" r:id="rId5"/>
     <sheet name="Products" sheetId="6" r:id="rId6"/>
   </sheets>
@@ -438,7 +438,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1197613-8BAE-49C4-AF59-A92BDA3CC00F}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
@@ -559,7 +559,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDE1ED40-DAA8-48CE-9AA7-CB5361C29315}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>